<commit_message>
added part 2 c plots
</commit_message>
<xml_diff>
--- a/part2/Table_Simulation-values.xlsx
+++ b/part2/Table_Simulation-values.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\icnas3.cc.ic.ac.uk\nmd16\ComputationalAerodynamicsSandbox\aca-docker\files\coursework\part2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ComputationalAerodynamicsSandbox\part2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41A60183-965F-4885-93ED-359C95444AD4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7AF980C-E896-451B-84CE-55A197CBE5A6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="705" yWindow="705" windowWidth="21600" windowHeight="11925" xr2:uid="{7CD09BEF-C2A4-47C3-97B4-6A618032A7ED}"/>
+    <workbookView xWindow="-1875" yWindow="2835" windowWidth="21600" windowHeight="11925" xr2:uid="{7CD09BEF-C2A4-47C3-97B4-6A618032A7ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -576,7 +576,7 @@
   <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -795,7 +795,7 @@
         <v>29</v>
       </c>
       <c r="F20">
-        <v>130.19999999999999</v>
+        <v>102.9</v>
       </c>
       <c r="G20" t="s">
         <v>26</v>
@@ -807,7 +807,7 @@
       </c>
       <c r="F21" s="1">
         <f>F24*F20</f>
-        <v>130.12068567788626</v>
+        <v>102.83731610026496</v>
       </c>
       <c r="G21" t="s">
         <v>26</v>
@@ -819,7 +819,7 @@
       </c>
       <c r="F22" s="1">
         <f>F25*F20</f>
-        <v>4.5439144706656212</v>
+        <v>3.5911582106873463</v>
       </c>
       <c r="G22" t="s">
         <v>26</v>
@@ -905,7 +905,7 @@
         <v>39</v>
       </c>
       <c r="F30" s="5">
-        <v>0.15243999999999999</v>
+        <v>1</v>
       </c>
       <c r="G30" s="5" t="s">
         <v>17</v>
@@ -917,7 +917,7 @@
       </c>
       <c r="F31" s="3">
         <f>(F14*F20*F30)/F2</f>
-        <v>2.4313417799999999E-5</v>
+        <v>1.2605250000000001E-4</v>
       </c>
       <c r="G31" t="s">
         <v>46</v>
@@ -952,7 +952,7 @@
       </c>
       <c r="F34">
         <f>0.5*F33*F14*F20*F20</f>
-        <v>38.889967479611492</v>
+        <v>24.29105408911218</v>
       </c>
       <c r="G34" t="s">
         <v>47</v>
@@ -964,7 +964,7 @@
       </c>
       <c r="F35">
         <f>SQRT(F34/F14)</f>
-        <v>5.6344398326944871</v>
+        <v>4.4530250290649986</v>
       </c>
       <c r="G35" t="s">
         <v>26</v>
@@ -987,7 +987,7 @@
       </c>
       <c r="F37" s="6">
         <f>F36*F31/F14/F35*2</f>
-        <v>6.3406193802437459E-6</v>
+        <v>4.1594196931538617E-5</v>
       </c>
       <c r="G37" t="s">
         <v>17</v>
@@ -1002,7 +1002,7 @@
       </c>
       <c r="F38" s="6">
         <f>0.37*F30/F32^0.2</f>
-        <v>3.5587760909247439E-3</v>
+        <v>2.3345421745767148E-2</v>
       </c>
       <c r="G38" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
added good and bad mesh images
</commit_message>
<xml_diff>
--- a/part2/Table_Simulation-values.xlsx
+++ b/part2/Table_Simulation-values.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ComputationalAerodynamicsSandbox\part2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7AF980C-E896-451B-84CE-55A197CBE5A6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69E799BC-BB61-41EB-82EC-00199CFF2AA4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1875" yWindow="2835" windowWidth="21600" windowHeight="11925" xr2:uid="{7CD09BEF-C2A4-47C3-97B4-6A618032A7ED}"/>
+    <workbookView xWindow="0" yWindow="1815" windowWidth="21600" windowHeight="11925" xr2:uid="{7CD09BEF-C2A4-47C3-97B4-6A618032A7ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -576,7 +576,7 @@
   <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -975,7 +975,7 @@
         <v>45</v>
       </c>
       <c r="F36">
-        <v>0.9</v>
+        <v>0.25</v>
       </c>
       <c r="G36" t="s">
         <v>7</v>
@@ -987,7 +987,7 @@
       </c>
       <c r="F37" s="6">
         <f>F36*F31/F14/F35*2</f>
-        <v>4.1594196931538617E-5</v>
+        <v>1.1553943592094059E-5</v>
       </c>
       <c r="G37" t="s">
         <v>17</v>

</xml_diff>